<commit_message>
Added dim button after start and fix data saved that did not actually save and added fclose
</commit_message>
<xml_diff>
--- a/sketch_180419a/coeffs.xlsx
+++ b/sketch_180419a/coeffs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD19820-9860-4BE0-BB52-321FDDF3F91A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263BBD04-1211-4872-80AA-01A76F95C388}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
   <si>
     <t>JJ</t>
   </si>
@@ -29,6 +29,15 @@
   </si>
   <si>
     <t>1 (2)</t>
+  </si>
+  <si>
+    <t>REALIZED TIMING ISSUE</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Percent Off</t>
   </si>
 </sst>
 </file>
@@ -64,10 +73,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -349,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="M7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="V12" sqref="U12:V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -360,7 +372,7 @@
     <col min="1" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -388,8 +400,26 @@
       <c r="K1" s="1">
         <v>-4.8446999999999996</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q1" s="1">
+        <v>1</v>
+      </c>
+      <c r="R1" s="1">
+        <v>1.075</v>
+      </c>
+      <c r="S1" s="1">
+        <v>-4.1909999999999998</v>
+      </c>
+      <c r="U1" s="1">
+        <v>1</v>
+      </c>
+      <c r="V1" s="1">
+        <v>1.0780000000000001</v>
+      </c>
+      <c r="W1" s="1">
+        <v>-3.5259999999999998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -417,8 +447,35 @@
       <c r="K2" s="1">
         <v>-4.1909999999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1.075</v>
+      </c>
+      <c r="O2" s="1">
+        <v>-4.1909999999999998</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>2</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1.105</v>
+      </c>
+      <c r="S2" s="1">
+        <v>-4.7290000000000001</v>
+      </c>
+      <c r="U2" s="1">
+        <v>2</v>
+      </c>
+      <c r="V2" s="1">
+        <v>1.105</v>
+      </c>
+      <c r="W2" s="1">
+        <v>-4.7290000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -437,8 +494,26 @@
       <c r="G3" s="1">
         <v>-3.641</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q3" s="1">
+        <v>3</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1.103</v>
+      </c>
+      <c r="S3" s="1">
+        <v>-4.9950000000000001</v>
+      </c>
+      <c r="U3" s="1">
+        <v>3</v>
+      </c>
+      <c r="V3" s="1">
+        <v>1.103</v>
+      </c>
+      <c r="W3" s="1">
+        <v>-4.9950000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -457,8 +532,20 @@
       <c r="G4" s="1">
         <v>-4.3019999999999996</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q4" s="1">
+        <v>4</v>
+      </c>
+      <c r="R4" s="1">
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="S4" s="1">
+        <v>-5.085</v>
+      </c>
+      <c r="U4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="E5" s="1">
         <v>4</v>
       </c>
@@ -477,8 +564,35 @@
       <c r="K5" s="1">
         <v>-5.085</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M5" s="1">
+        <v>4</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="O5" s="1">
+        <v>-5.085</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>5</v>
+      </c>
+      <c r="R5" s="1">
+        <v>1.069</v>
+      </c>
+      <c r="S5" s="1">
+        <v>-3.0390000000000001</v>
+      </c>
+      <c r="U5" s="1">
+        <v>5</v>
+      </c>
+      <c r="V5" s="1">
+        <v>1.069</v>
+      </c>
+      <c r="W5" s="1">
+        <v>-3.0390000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -512,8 +626,36 @@
         <f>AVERAGE(K1:K5)</f>
         <v>-4.7069000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M6" s="1">
+        <f>AVERAGE(M2:M5)</f>
+        <v>2.5</v>
+      </c>
+      <c r="N6" s="1">
+        <f>AVERAGE(N2:N5)</f>
+        <v>1.0905</v>
+      </c>
+      <c r="O6" s="1">
+        <f>AVERAGE(O2:O5)</f>
+        <v>-4.6379999999999999</v>
+      </c>
+      <c r="R6" s="1">
+        <f>AVERAGE(R1:R5)</f>
+        <v>1.0915999999999999</v>
+      </c>
+      <c r="S6" s="1">
+        <f>AVERAGE(S1:S5)</f>
+        <v>-4.4077999999999999</v>
+      </c>
+      <c r="V6" s="1">
+        <f>AVERAGE(V1:V5)</f>
+        <v>1.0887499999999999</v>
+      </c>
+      <c r="W6" s="1">
+        <f>AVERAGE(W1:W5)</f>
+        <v>-4.0722500000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="E8" s="1" t="s">
         <v>0</v>
       </c>
@@ -523,8 +665,15 @@
       <c r="G8" s="1">
         <v>-4.8446999999999996</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="R8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="E9" s="1">
         <v>1</v>
       </c>
@@ -534,8 +683,29 @@
       <c r="G9" s="1">
         <v>-4.1909999999999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N9" s="1">
+        <v>1</v>
+      </c>
+      <c r="O9" s="1">
+        <v>1.0780000000000001</v>
+      </c>
+      <c r="P9" s="1">
+        <v>-3.5259999999999998</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0.23039999999999999</v>
+      </c>
+      <c r="T9" s="1">
+        <v>1</v>
+      </c>
+      <c r="U9" s="1">
+        <v>1.141</v>
+      </c>
+      <c r="V9" s="1">
+        <v>-5.6740000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="E10" s="1">
         <v>2</v>
       </c>
@@ -545,8 +715,29 @@
       <c r="G10" s="1">
         <v>-3.641</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N10" s="1">
+        <v>2</v>
+      </c>
+      <c r="O10" s="1">
+        <v>1.1140000000000001</v>
+      </c>
+      <c r="P10" s="1">
+        <v>-5.0030000000000001</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0.1739</v>
+      </c>
+      <c r="T10" s="1">
+        <v>2</v>
+      </c>
+      <c r="U10" s="1">
+        <v>1.1140000000000001</v>
+      </c>
+      <c r="V10" s="1">
+        <v>-5.0030000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="E11" s="1">
         <v>3</v>
       </c>
@@ -556,8 +747,29 @@
       <c r="G11" s="1">
         <v>-4.3019999999999996</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N11" s="1">
+        <v>3</v>
+      </c>
+      <c r="O11" s="1">
+        <v>1.1120000000000001</v>
+      </c>
+      <c r="P11" s="1">
+        <v>-5.2359999999999998</v>
+      </c>
+      <c r="R11" s="1">
+        <v>1.0581</v>
+      </c>
+      <c r="T11" s="1">
+        <v>3</v>
+      </c>
+      <c r="U11" s="1">
+        <v>1.1120000000000001</v>
+      </c>
+      <c r="V11" s="1">
+        <v>-5.2359999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="E12" s="1">
         <v>4</v>
       </c>
@@ -567,8 +779,29 @@
       <c r="G12" s="1">
         <v>-5.085</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N12" s="1">
+        <v>4</v>
+      </c>
+      <c r="O12" s="1">
+        <v>1.1679999999999999</v>
+      </c>
+      <c r="P12" s="1">
+        <v>-6.8390000000000004</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0.44140000000000001</v>
+      </c>
+      <c r="T12" s="1">
+        <v>4</v>
+      </c>
+      <c r="U12" s="1">
+        <v>1.1679999999999999</v>
+      </c>
+      <c r="V12" s="1">
+        <v>-6.8390000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="E13" s="1" t="s">
         <v>2</v>
       </c>
@@ -578,8 +811,29 @@
       <c r="G13" s="1">
         <v>-4.8029999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N13" s="1">
+        <v>5</v>
+      </c>
+      <c r="O13" s="1">
+        <v>1.0740000000000001</v>
+      </c>
+      <c r="P13" s="1">
+        <v>-3.1970000000000001</v>
+      </c>
+      <c r="R13" s="1">
+        <v>0.44409999999999999</v>
+      </c>
+      <c r="T13" s="1">
+        <v>5</v>
+      </c>
+      <c r="U13" s="1">
+        <v>1.0740000000000001</v>
+      </c>
+      <c r="V13" s="1">
+        <v>-3.1970000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="E14" s="1" t="s">
         <v>1</v>
       </c>
@@ -590,6 +844,32 @@
       <c r="G14" s="1">
         <f>AVERAGE(G8:G13)</f>
         <v>-4.477783333333333</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O14" s="1">
+        <f>AVERAGE(O9:O13)</f>
+        <v>1.1092</v>
+      </c>
+      <c r="P14" s="1">
+        <f>AVERAGE(P9:P13)</f>
+        <v>-4.7601999999999993</v>
+      </c>
+      <c r="R14" s="1">
+        <f>AVERAGE(R9:R13)</f>
+        <v>0.46958</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U14" s="1">
+        <f>AVERAGE(U9:U13)</f>
+        <v>1.1217999999999999</v>
+      </c>
+      <c r="V14" s="1">
+        <f>AVERAGE(V9:V13)</f>
+        <v>-5.1898</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reorganize files and extract only important ones. Add error reporting script and rename Post_Report_Run.m
</commit_message>
<xml_diff>
--- a/sketch_180419a/coeffs.xlsx
+++ b/sketch_180419a/coeffs.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263BBD04-1211-4872-80AA-01A76F95C388}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6FC07F-38EE-4B85-BE81-CF1E245D0600}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="23">
   <si>
     <t>JJ</t>
   </si>
@@ -37,14 +37,68 @@
     <t>Mean</t>
   </si>
   <si>
-    <t>Percent Off</t>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>Sensor No.</t>
+  </si>
+  <si>
+    <t>Attempt1</t>
+  </si>
+  <si>
+    <t>Attempt2</t>
+  </si>
+  <si>
+    <t>Attempt3</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>Trial1</t>
+  </si>
+  <si>
+    <t>Trial2</t>
+  </si>
+  <si>
+    <t>Trial3</t>
+  </si>
+  <si>
+    <t>Ave</t>
+  </si>
+  <si>
+    <t>Slope p1</t>
+  </si>
+  <si>
+    <t>Offset p2</t>
+  </si>
+  <si>
+    <t>Ave Percent Off</t>
+  </si>
+  <si>
+    <t>Min Percent Off</t>
+  </si>
+  <si>
+    <t>Max Percent Off</t>
+  </si>
+  <si>
+    <t>Ave Abs Off</t>
+  </si>
+  <si>
+    <t>Min Abs Off</t>
+  </si>
+  <si>
+    <t>Max Abs Off</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,16 +106,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -69,17 +160,93 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -361,18 +528,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:BC30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="V12" sqref="U12:V13"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AM27" sqref="AM27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="2" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="1"/>
+    <col min="5" max="6" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" style="1"/>
+    <col min="9" max="10" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.109375" style="1"/>
+    <col min="17" max="18" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.109375" style="1"/>
+    <col min="21" max="21" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="31" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="8.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -400,6 +590,15 @@
       <c r="K1" s="1">
         <v>-4.8446999999999996</v>
       </c>
+      <c r="M1" s="1">
+        <v>1</v>
+      </c>
+      <c r="N1" s="1">
+        <v>1.075</v>
+      </c>
+      <c r="O1" s="1">
+        <v>-4.1909999999999998</v>
+      </c>
       <c r="Q1" s="1">
         <v>1</v>
       </c>
@@ -412,14 +611,28 @@
       <c r="U1" s="1">
         <v>1</v>
       </c>
-      <c r="V1" s="1">
+      <c r="V1" s="2">
         <v>1.0780000000000001</v>
       </c>
-      <c r="W1" s="1">
+      <c r="W1" s="2">
         <v>-3.5259999999999998</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AG1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AM1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="12"/>
+    </row>
+    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -448,21 +661,15 @@
         <v>-4.1909999999999998</v>
       </c>
       <c r="M2" s="1">
-        <v>1</v>
-      </c>
-      <c r="N2" s="1">
-        <v>1.075</v>
-      </c>
-      <c r="O2" s="1">
-        <v>-4.1909999999999998</v>
+        <v>2</v>
       </c>
       <c r="Q2" s="1">
         <v>2</v>
       </c>
-      <c r="R2" s="1">
+      <c r="R2" s="2">
         <v>1.105</v>
       </c>
-      <c r="S2" s="1">
+      <c r="S2" s="2">
         <v>-4.7290000000000001</v>
       </c>
       <c r="U2" s="1">
@@ -474,8 +681,38 @@
       <c r="W2" s="1">
         <v>-4.7290000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AG2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AM2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AN2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ2" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -494,13 +731,16 @@
       <c r="G3" s="1">
         <v>-3.641</v>
       </c>
+      <c r="M3" s="1">
+        <v>3</v>
+      </c>
       <c r="Q3" s="1">
         <v>3</v>
       </c>
-      <c r="R3" s="1">
+      <c r="R3" s="2">
         <v>1.103</v>
       </c>
-      <c r="S3" s="1">
+      <c r="S3" s="2">
         <v>-4.9950000000000001</v>
       </c>
       <c r="U3" s="1">
@@ -512,8 +752,40 @@
       <c r="W3" s="1">
         <v>-4.9950000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AG3" s="6">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="8">
+        <v>1.0780000000000001</v>
+      </c>
+      <c r="AI3" s="7">
+        <v>1.141</v>
+      </c>
+      <c r="AJ3" s="7">
+        <v>1.121</v>
+      </c>
+      <c r="AK3" s="7">
+        <f>AVERAGE(AH3:AJ3)</f>
+        <v>1.1133333333333335</v>
+      </c>
+      <c r="AM3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AN3" s="8">
+        <v>-3.5259999999999998</v>
+      </c>
+      <c r="AO3" s="7">
+        <v>-5.6740000000000004</v>
+      </c>
+      <c r="AP3" s="7">
+        <v>-5.1840000000000002</v>
+      </c>
+      <c r="AQ3" s="7">
+        <f>AVERAGE(AN3:AP3)</f>
+        <v>-4.7946666666666671</v>
+      </c>
+    </row>
+    <row r="4" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -532,6 +804,15 @@
       <c r="G4" s="1">
         <v>-4.3019999999999996</v>
       </c>
+      <c r="M4" s="1">
+        <v>4</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="O4" s="1">
+        <v>-5.085</v>
+      </c>
       <c r="Q4" s="1">
         <v>4</v>
       </c>
@@ -544,8 +825,40 @@
       <c r="U4" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AG4" s="6">
+        <v>2</v>
+      </c>
+      <c r="AH4" s="7">
+        <v>1.1140000000000001</v>
+      </c>
+      <c r="AI4" s="7">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="AJ4" s="8">
+        <v>1.0920000000000001</v>
+      </c>
+      <c r="AK4" s="7">
+        <f>AVERAGE(AH4:AJ4)</f>
+        <v>1.1086666666666667</v>
+      </c>
+      <c r="AM4" s="7">
+        <v>2</v>
+      </c>
+      <c r="AN4" s="7">
+        <v>-5.0030000000000001</v>
+      </c>
+      <c r="AO4" s="7">
+        <v>-5.1689999999999996</v>
+      </c>
+      <c r="AP4" s="8">
+        <v>-4.4569999999999999</v>
+      </c>
+      <c r="AQ4" s="7">
+        <f>AVERAGE(AN4:AP4)</f>
+        <v>-4.8763333333333341</v>
+      </c>
+    </row>
+    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
       <c r="E5" s="1">
         <v>4</v>
       </c>
@@ -565,21 +878,15 @@
         <v>-5.085</v>
       </c>
       <c r="M5" s="1">
-        <v>4</v>
-      </c>
-      <c r="N5" s="1">
-        <v>1.1060000000000001</v>
-      </c>
-      <c r="O5" s="1">
-        <v>-5.085</v>
+        <v>5</v>
       </c>
       <c r="Q5" s="1">
         <v>5</v>
       </c>
-      <c r="R5" s="1">
+      <c r="R5" s="2">
         <v>1.069</v>
       </c>
-      <c r="S5" s="1">
+      <c r="S5" s="2">
         <v>-3.0390000000000001</v>
       </c>
       <c r="U5" s="1">
@@ -591,8 +898,40 @@
       <c r="W5" s="1">
         <v>-3.0390000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AG5" s="6">
+        <v>3</v>
+      </c>
+      <c r="AH5" s="7">
+        <v>1.1120000000000001</v>
+      </c>
+      <c r="AI5" s="8">
+        <v>1.095</v>
+      </c>
+      <c r="AJ5" s="7">
+        <v>1.113</v>
+      </c>
+      <c r="AK5" s="7">
+        <f>AVERAGE(AH5:AJ5)</f>
+        <v>1.1066666666666667</v>
+      </c>
+      <c r="AM5" s="7">
+        <v>3</v>
+      </c>
+      <c r="AN5" s="7">
+        <v>-5.2359999999999998</v>
+      </c>
+      <c r="AO5" s="8">
+        <v>-4.5039999999999996</v>
+      </c>
+      <c r="AP5" s="7">
+        <v>-5.1219999999999999</v>
+      </c>
+      <c r="AQ5" s="7">
+        <f>AVERAGE(AN5:AP5)</f>
+        <v>-4.9539999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -626,17 +965,19 @@
         <f>AVERAGE(K1:K5)</f>
         <v>-4.7069000000000001</v>
       </c>
-      <c r="M6" s="1">
-        <f>AVERAGE(M2:M5)</f>
-        <v>2.5</v>
+      <c r="M6" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="N6" s="1">
-        <f>AVERAGE(N2:N5)</f>
+        <f>AVERAGE(N1:N4)</f>
         <v>1.0905</v>
       </c>
       <c r="O6" s="1">
-        <f>AVERAGE(O2:O5)</f>
+        <f>AVERAGE(O1:O4)</f>
         <v>-4.6379999999999999</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="R6" s="1">
         <f>AVERAGE(R1:R5)</f>
@@ -646,6 +987,9 @@
         <f>AVERAGE(S1:S5)</f>
         <v>-4.4077999999999999</v>
       </c>
+      <c r="U6" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="V6" s="1">
         <f>AVERAGE(V1:V5)</f>
         <v>1.0887499999999999</v>
@@ -654,8 +998,74 @@
         <f>AVERAGE(W1:W5)</f>
         <v>-4.0722500000000004</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AG6" s="6">
+        <v>4</v>
+      </c>
+      <c r="AH6" s="7">
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="AI6" s="8">
+        <v>1.1679999999999999</v>
+      </c>
+      <c r="AJ6" s="7">
+        <v>1.109</v>
+      </c>
+      <c r="AK6" s="7">
+        <f>AVERAGE(AH6:AJ6)</f>
+        <v>1.1276666666666666</v>
+      </c>
+      <c r="AM6" s="7">
+        <v>4</v>
+      </c>
+      <c r="AN6" s="7">
+        <v>-5.085</v>
+      </c>
+      <c r="AO6" s="8">
+        <v>-6.8390000000000004</v>
+      </c>
+      <c r="AP6" s="7">
+        <v>-5.0380000000000003</v>
+      </c>
+      <c r="AQ6" s="7">
+        <f>AVERAGE(AN6:AP6)</f>
+        <v>-5.6539999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AG7" s="6">
+        <v>5</v>
+      </c>
+      <c r="AH7" s="11">
+        <v>1.0740000000000001</v>
+      </c>
+      <c r="AI7" s="7">
+        <v>1.085</v>
+      </c>
+      <c r="AJ7" s="7">
+        <v>1.089</v>
+      </c>
+      <c r="AK7" s="9">
+        <f>AVERAGE(AH7:AJ7)</f>
+        <v>1.0826666666666667</v>
+      </c>
+      <c r="AM7" s="7">
+        <v>5</v>
+      </c>
+      <c r="AN7" s="11">
+        <v>-3.1970000000000001</v>
+      </c>
+      <c r="AO7" s="7">
+        <v>-3.8929999999999998</v>
+      </c>
+      <c r="AP7" s="7">
+        <v>-4.0359999999999996</v>
+      </c>
+      <c r="AQ7" s="9">
+        <f>AVERAGE(AN7:AP7)</f>
+        <v>-3.7086666666666663</v>
+      </c>
+    </row>
+    <row r="8" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E8" s="1" t="s">
         <v>0</v>
       </c>
@@ -665,15 +1075,23 @@
       <c r="G8" s="1">
         <v>-4.8446999999999996</v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O8" s="2"/>
-      <c r="R8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="M8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="3"/>
+      <c r="AK8" s="10">
+        <f>AVERAGE(AK3:AK7)</f>
+        <v>1.1077999999999999</v>
+      </c>
+      <c r="AQ8" s="10">
+        <f>AVERAGE(AQ3:AQ7)</f>
+        <v>-4.797533333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
       <c r="E9" s="1">
         <v>1</v>
       </c>
@@ -683,29 +1101,47 @@
       <c r="G9" s="1">
         <v>-4.1909999999999998</v>
       </c>
+      <c r="L9" s="1">
+        <v>0.23039999999999999</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1</v>
+      </c>
       <c r="N9" s="1">
-        <v>1</v>
+        <v>1.0780000000000001</v>
       </c>
       <c r="O9" s="1">
-        <v>1.0780000000000001</v>
-      </c>
-      <c r="P9" s="1">
         <v>-3.5259999999999998</v>
       </c>
-      <c r="R9" s="1">
-        <v>0.23039999999999999</v>
-      </c>
-      <c r="T9" s="1">
-        <v>1</v>
+      <c r="Q9" s="1">
+        <v>1</v>
+      </c>
+      <c r="R9" s="2">
+        <v>1.141</v>
+      </c>
+      <c r="S9" s="2">
+        <v>-5.6740000000000004</v>
       </c>
       <c r="U9" s="1">
-        <v>1.141</v>
-      </c>
-      <c r="V9" s="1">
-        <v>-5.6740000000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="V9" s="2">
+        <v>1.121</v>
+      </c>
+      <c r="W9" s="2">
+        <v>-5.1840000000000002</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="4">
+        <v>1.121</v>
+      </c>
+      <c r="AA9" s="4">
+        <v>-5.1840000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
       <c r="E10" s="1">
         <v>2</v>
       </c>
@@ -715,29 +1151,75 @@
       <c r="G10" s="1">
         <v>-3.641</v>
       </c>
+      <c r="L10" s="1">
+        <v>0.1739</v>
+      </c>
+      <c r="M10" s="1">
+        <v>2</v>
+      </c>
       <c r="N10" s="1">
-        <v>2</v>
+        <v>1.1140000000000001</v>
       </c>
       <c r="O10" s="1">
+        <v>-5.0030000000000001</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>2</v>
+      </c>
+      <c r="R10" s="1">
         <v>1.1140000000000001</v>
       </c>
-      <c r="P10" s="1">
+      <c r="S10" s="1">
         <v>-5.0030000000000001</v>
       </c>
-      <c r="R10" s="1">
-        <v>0.1739</v>
-      </c>
-      <c r="T10" s="1">
-        <v>2</v>
-      </c>
       <c r="U10" s="1">
+        <v>2</v>
+      </c>
+      <c r="V10" s="1">
         <v>1.1140000000000001</v>
       </c>
-      <c r="V10" s="1">
+      <c r="W10" s="1">
         <v>-5.0030000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Y10" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>1.1140000000000001</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>-5.0030000000000001</v>
+      </c>
+      <c r="AG10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH10" s="12"/>
+      <c r="AI10" s="12"/>
+      <c r="AJ10" s="12"/>
+      <c r="AK10" s="12"/>
+      <c r="AM10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="AN10" s="12"/>
+      <c r="AO10" s="12"/>
+      <c r="AP10" s="12"/>
+      <c r="AQ10" s="12"/>
+      <c r="AS10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AT10" s="12"/>
+      <c r="AU10" s="12"/>
+      <c r="AV10" s="12"/>
+      <c r="AW10" s="12"/>
+      <c r="AY10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="AZ10" s="12"/>
+      <c r="BA10" s="12"/>
+      <c r="BB10" s="12"/>
+      <c r="BC10" s="12"/>
+    </row>
+    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
       <c r="E11" s="1">
         <v>3</v>
       </c>
@@ -747,29 +1229,107 @@
       <c r="G11" s="1">
         <v>-4.3019999999999996</v>
       </c>
+      <c r="L11" s="1">
+        <v>1.0581</v>
+      </c>
+      <c r="M11" s="1">
+        <v>3</v>
+      </c>
       <c r="N11" s="1">
-        <v>3</v>
+        <v>1.1120000000000001</v>
       </c>
       <c r="O11" s="1">
+        <v>-5.2359999999999998</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>3</v>
+      </c>
+      <c r="R11" s="1">
         <v>1.1120000000000001</v>
       </c>
-      <c r="P11" s="1">
+      <c r="S11" s="1">
         <v>-5.2359999999999998</v>
       </c>
-      <c r="R11" s="1">
-        <v>1.0581</v>
-      </c>
-      <c r="T11" s="1">
-        <v>3</v>
-      </c>
       <c r="U11" s="1">
+        <v>3</v>
+      </c>
+      <c r="V11" s="1">
         <v>1.1120000000000001</v>
       </c>
-      <c r="V11" s="1">
+      <c r="W11" s="1">
         <v>-5.2359999999999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Y11" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>1.1120000000000001</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>-5.2359999999999998</v>
+      </c>
+      <c r="AG11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AM11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AN11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AT11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AU11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AW11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AY11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AZ11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="BA11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="BB11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BC11" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:55" x14ac:dyDescent="0.3">
       <c r="E12" s="1">
         <v>4</v>
       </c>
@@ -779,29 +1339,87 @@
       <c r="G12" s="1">
         <v>-5.085</v>
       </c>
-      <c r="N12" s="1">
-        <v>4</v>
-      </c>
-      <c r="O12" s="1">
+      <c r="L12" s="1">
+        <v>0.44140000000000001</v>
+      </c>
+      <c r="M12" s="1">
+        <v>4</v>
+      </c>
+      <c r="N12" s="5">
         <v>1.1679999999999999</v>
       </c>
-      <c r="P12" s="1">
+      <c r="O12" s="5">
         <v>-6.8390000000000004</v>
       </c>
+      <c r="Q12" s="1">
+        <v>4</v>
+      </c>
       <c r="R12" s="1">
-        <v>0.44140000000000001</v>
-      </c>
-      <c r="T12" s="1">
-        <v>4</v>
+        <v>1.1679999999999999</v>
+      </c>
+      <c r="S12" s="1">
+        <v>-6.8390000000000004</v>
       </c>
       <c r="U12" s="1">
+        <v>4</v>
+      </c>
+      <c r="V12" s="1">
         <v>1.1679999999999999</v>
       </c>
-      <c r="V12" s="1">
+      <c r="W12" s="1">
         <v>-6.8390000000000004</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Y12" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>1.109</v>
+      </c>
+      <c r="AA12" s="2">
+        <v>-5.0380000000000003</v>
+      </c>
+      <c r="AG12" s="6">
+        <v>1</v>
+      </c>
+      <c r="AH12" s="8"/>
+      <c r="AI12" s="7"/>
+      <c r="AJ12" s="7"/>
+      <c r="AK12" s="7" t="e">
+        <f>AVERAGE(AH12:AJ12)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM12" s="6">
+        <v>1</v>
+      </c>
+      <c r="AN12" s="8"/>
+      <c r="AO12" s="7"/>
+      <c r="AP12" s="7"/>
+      <c r="AQ12" s="7" t="e">
+        <f>AVERAGE(AN12:AP12)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS12" s="6">
+        <v>1</v>
+      </c>
+      <c r="AT12" s="8"/>
+      <c r="AU12" s="7"/>
+      <c r="AV12" s="7"/>
+      <c r="AW12" s="7" t="e">
+        <f>AVERAGE(AT12:AV12)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AY12" s="6">
+        <v>1</v>
+      </c>
+      <c r="AZ12" s="8"/>
+      <c r="BA12" s="7"/>
+      <c r="BB12" s="7"/>
+      <c r="BC12" s="7" t="e">
+        <f>AVERAGE(AZ12:BB12)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:55" x14ac:dyDescent="0.3">
       <c r="E13" s="1" t="s">
         <v>2</v>
       </c>
@@ -811,29 +1429,87 @@
       <c r="G13" s="1">
         <v>-4.8029999999999999</v>
       </c>
+      <c r="L13" s="1">
+        <v>0.44409999999999999</v>
+      </c>
+      <c r="M13" s="1">
+        <v>5</v>
+      </c>
       <c r="N13" s="1">
+        <v>1.0740000000000001</v>
+      </c>
+      <c r="O13" s="1">
+        <v>-3.1970000000000001</v>
+      </c>
+      <c r="Q13" s="1">
         <v>5</v>
       </c>
-      <c r="O13" s="1">
+      <c r="R13" s="1">
         <v>1.0740000000000001</v>
       </c>
-      <c r="P13" s="1">
+      <c r="S13" s="1">
         <v>-3.1970000000000001</v>
       </c>
-      <c r="R13" s="1">
-        <v>0.44409999999999999</v>
-      </c>
-      <c r="T13" s="1">
+      <c r="U13" s="1">
         <v>5</v>
       </c>
-      <c r="U13" s="1">
+      <c r="V13" s="1">
         <v>1.0740000000000001</v>
       </c>
-      <c r="V13" s="1">
+      <c r="W13" s="1">
         <v>-3.1970000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Y13" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>1.0740000000000001</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>-3.1970000000000001</v>
+      </c>
+      <c r="AG13" s="6">
+        <v>2</v>
+      </c>
+      <c r="AH13" s="7"/>
+      <c r="AI13" s="7"/>
+      <c r="AJ13" s="8"/>
+      <c r="AK13" s="7" t="e">
+        <f>AVERAGE(AH13:AJ13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM13" s="6">
+        <v>2</v>
+      </c>
+      <c r="AN13" s="7"/>
+      <c r="AO13" s="7"/>
+      <c r="AP13" s="8"/>
+      <c r="AQ13" s="7" t="e">
+        <f>AVERAGE(AN13:AP13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS13" s="6">
+        <v>2</v>
+      </c>
+      <c r="AT13" s="7"/>
+      <c r="AU13" s="7"/>
+      <c r="AV13" s="8"/>
+      <c r="AW13" s="7" t="e">
+        <f>AVERAGE(AT13:AV13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AY13" s="6">
+        <v>2</v>
+      </c>
+      <c r="AZ13" s="7"/>
+      <c r="BA13" s="7"/>
+      <c r="BB13" s="8"/>
+      <c r="BC13" s="7" t="e">
+        <f>AVERAGE(AZ13:BB13)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
       <c r="E14" s="1" t="s">
         <v>1</v>
       </c>
@@ -845,34 +1521,910 @@
         <f>AVERAGE(G8:G13)</f>
         <v>-4.477783333333333</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>4</v>
+      <c r="L14" s="1">
+        <f>AVERAGE(L9:L13)</f>
+        <v>0.46958</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N14" s="1">
+        <f>AVERAGE(N9:N13)</f>
+        <v>1.1092</v>
       </c>
       <c r="O14" s="1">
         <f>AVERAGE(O9:O13)</f>
-        <v>1.1092</v>
-      </c>
-      <c r="P14" s="1">
-        <f>AVERAGE(P9:P13)</f>
         <v>-4.7601999999999993</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="R14" s="1">
         <f>AVERAGE(R9:R13)</f>
-        <v>0.46958</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U14" s="1">
-        <f>AVERAGE(U9:U13)</f>
         <v>1.1217999999999999</v>
+      </c>
+      <c r="S14" s="1">
+        <f>AVERAGE(S9:S13)</f>
+        <v>-5.1898</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="V14" s="1">
         <f>AVERAGE(V9:V13)</f>
-        <v>-5.1898</v>
+        <v>1.1178000000000001</v>
+      </c>
+      <c r="W14" s="1">
+        <f>AVERAGE(W9:W13)</f>
+        <v>-5.0918000000000001</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z14" s="1">
+        <f>AVERAGE(Z9:Z13)</f>
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="AA14" s="1">
+        <f>AVERAGE(AA9:AA13)</f>
+        <v>-4.7316000000000003</v>
+      </c>
+      <c r="AG14" s="6">
+        <v>3</v>
+      </c>
+      <c r="AH14" s="7">
+        <v>0.81169999999999998</v>
+      </c>
+      <c r="AI14" s="8"/>
+      <c r="AJ14" s="7"/>
+      <c r="AK14" s="7">
+        <f>AVERAGE(AH14:AJ14)</f>
+        <v>0.81169999999999998</v>
+      </c>
+      <c r="AM14" s="6">
+        <v>3</v>
+      </c>
+      <c r="AN14" s="7">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="AO14" s="8"/>
+      <c r="AP14" s="7"/>
+      <c r="AQ14" s="7">
+        <f>AVERAGE(AN14:AP14)</f>
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="AS14" s="6">
+        <v>3</v>
+      </c>
+      <c r="AT14" s="7">
+        <v>0.29420000000000002</v>
+      </c>
+      <c r="AU14" s="8"/>
+      <c r="AV14" s="7"/>
+      <c r="AW14" s="7">
+        <f>AVERAGE(AT14:AV14)</f>
+        <v>0.29420000000000002</v>
+      </c>
+      <c r="AY14" s="6">
+        <v>3</v>
+      </c>
+      <c r="AZ14" s="7">
+        <v>1.01E-2</v>
+      </c>
+      <c r="BA14" s="8"/>
+      <c r="BB14" s="7"/>
+      <c r="BC14" s="7">
+        <f>AVERAGE(AZ14:BB14)</f>
+        <v>1.01E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="AG15" s="6">
+        <v>4</v>
+      </c>
+      <c r="AH15" s="7"/>
+      <c r="AI15" s="8"/>
+      <c r="AJ15" s="7"/>
+      <c r="AK15" s="7" t="e">
+        <f>AVERAGE(AH15:AJ15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM15" s="6">
+        <v>4</v>
+      </c>
+      <c r="AN15" s="7"/>
+      <c r="AO15" s="8"/>
+      <c r="AP15" s="7"/>
+      <c r="AQ15" s="7" t="e">
+        <f>AVERAGE(AN15:AP15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS15" s="6">
+        <v>4</v>
+      </c>
+      <c r="AT15" s="7"/>
+      <c r="AU15" s="8"/>
+      <c r="AV15" s="7"/>
+      <c r="AW15" s="7" t="e">
+        <f>AVERAGE(AT15:AV15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AY15" s="6">
+        <v>4</v>
+      </c>
+      <c r="AZ15" s="7"/>
+      <c r="BA15" s="8"/>
+      <c r="BB15" s="7"/>
+      <c r="BC15" s="7" t="e">
+        <f>AVERAGE(AZ15:BB15)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="AG16" s="6">
+        <v>5</v>
+      </c>
+      <c r="AH16" s="8">
+        <v>0.66180000000000005</v>
+      </c>
+      <c r="AI16" s="7">
+        <v>0.25019999999999998</v>
+      </c>
+      <c r="AJ16" s="7">
+        <v>0.23930000000000001</v>
+      </c>
+      <c r="AK16" s="7">
+        <f>AVERAGE(AH16:AJ16)</f>
+        <v>0.38376666666666664</v>
+      </c>
+      <c r="AM16" s="6">
+        <v>5</v>
+      </c>
+      <c r="AN16" s="8">
+        <v>4.9178999999999998E-4</v>
+      </c>
+      <c r="AO16" s="7">
+        <v>1.6775000000000001E-4</v>
+      </c>
+      <c r="AP16" s="7">
+        <v>8.6789999999999994E-6</v>
+      </c>
+      <c r="AQ16" s="7">
+        <f>AVERAGE(AN16:AP16)</f>
+        <v>2.2273966666666668E-4</v>
+      </c>
+      <c r="AS16" s="6">
+        <v>5</v>
+      </c>
+      <c r="AT16" s="8">
+        <v>0.255</v>
+      </c>
+      <c r="AU16" s="7">
+        <v>8.8700000000000001E-2</v>
+      </c>
+      <c r="AV16" s="7">
+        <v>8.3500000000000005E-2</v>
+      </c>
+      <c r="AW16" s="7">
+        <f>AVERAGE(AT16:AV16)</f>
+        <v>0.1424</v>
+      </c>
+      <c r="AY16" s="6">
+        <v>5</v>
+      </c>
+      <c r="AZ16" s="8">
+        <v>2.1667E-4</v>
+      </c>
+      <c r="BA16" s="7">
+        <v>6.9999999999999994E-5</v>
+      </c>
+      <c r="BB16" s="7">
+        <v>3.3332999999999999E-6</v>
+      </c>
+      <c r="BC16" s="7">
+        <f>AVERAGE(AZ16:BB16)</f>
+        <v>9.6667766666666663E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="13:49" x14ac:dyDescent="0.3">
+      <c r="M17" s="1">
+        <v>1</v>
+      </c>
+      <c r="N17" s="4">
+        <v>1.121</v>
+      </c>
+      <c r="O17" s="4">
+        <v>-5.1840000000000002</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>1</v>
+      </c>
+      <c r="R17" s="4">
+        <v>1.121</v>
+      </c>
+      <c r="S17" s="4">
+        <v>-5.1840000000000002</v>
+      </c>
+      <c r="U17" s="1">
+        <v>1</v>
+      </c>
+      <c r="V17" s="4">
+        <v>1.121</v>
+      </c>
+      <c r="W17" s="4">
+        <v>-5.1840000000000002</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="4">
+        <v>1.121</v>
+      </c>
+      <c r="AA17" s="4">
+        <v>-5.1840000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="13:49" x14ac:dyDescent="0.3">
+      <c r="M18" s="1">
+        <v>2</v>
+      </c>
+      <c r="N18" s="1">
+        <v>1.1140000000000001</v>
+      </c>
+      <c r="O18" s="1">
+        <v>-5.0030000000000001</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>2</v>
+      </c>
+      <c r="R18" s="2">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="S18" s="2">
+        <v>-5.1689999999999996</v>
+      </c>
+      <c r="U18" s="1">
+        <v>2</v>
+      </c>
+      <c r="V18" s="4">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="W18" s="4">
+        <v>-5.1689999999999996</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z18" s="2">
+        <v>1.0920000000000001</v>
+      </c>
+      <c r="AA18" s="2">
+        <v>-4.4569999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="13:49" x14ac:dyDescent="0.3">
+      <c r="M19" s="1">
+        <v>3</v>
+      </c>
+      <c r="N19" s="1">
+        <v>1.1120000000000001</v>
+      </c>
+      <c r="O19" s="1">
+        <v>-5.2359999999999998</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>3</v>
+      </c>
+      <c r="R19" s="1">
+        <v>1.1120000000000001</v>
+      </c>
+      <c r="S19" s="1">
+        <v>-5.2359999999999998</v>
+      </c>
+      <c r="U19" s="1">
+        <v>3</v>
+      </c>
+      <c r="V19" s="2">
+        <v>1.095</v>
+      </c>
+      <c r="W19" s="2">
+        <v>-4.5039999999999996</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z19" s="4">
+        <v>1.095</v>
+      </c>
+      <c r="AA19" s="4">
+        <v>-4.5039999999999996</v>
+      </c>
+      <c r="AG19" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH19" s="12"/>
+      <c r="AI19" s="12"/>
+      <c r="AJ19" s="12"/>
+      <c r="AK19" s="12"/>
+      <c r="AS19" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT19" s="12"/>
+      <c r="AU19" s="12"/>
+      <c r="AV19" s="12"/>
+      <c r="AW19" s="12"/>
+    </row>
+    <row r="20" spans="13:49" x14ac:dyDescent="0.3">
+      <c r="M20" s="1">
+        <v>4</v>
+      </c>
+      <c r="N20" s="4">
+        <v>1.109</v>
+      </c>
+      <c r="O20" s="4">
+        <v>-5.0380000000000003</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>4</v>
+      </c>
+      <c r="R20" s="4">
+        <v>1.109</v>
+      </c>
+      <c r="S20" s="4">
+        <v>-5.0380000000000003</v>
+      </c>
+      <c r="U20" s="1">
+        <v>4</v>
+      </c>
+      <c r="V20" s="4">
+        <v>1.109</v>
+      </c>
+      <c r="W20" s="4">
+        <v>-5.0380000000000003</v>
+      </c>
+      <c r="Y20" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z20" s="4">
+        <v>1.109</v>
+      </c>
+      <c r="AA20" s="4">
+        <v>-5.0380000000000003</v>
+      </c>
+      <c r="AG20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AT20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AU20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AW20" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="13:49" x14ac:dyDescent="0.3">
+      <c r="M21" s="1">
+        <v>5</v>
+      </c>
+      <c r="N21" s="5">
+        <v>1.085</v>
+      </c>
+      <c r="O21" s="5">
+        <v>-3.8929999999999998</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>5</v>
+      </c>
+      <c r="R21" s="4">
+        <v>1.085</v>
+      </c>
+      <c r="S21" s="4">
+        <v>-3.8929999999999998</v>
+      </c>
+      <c r="U21" s="1">
+        <v>5</v>
+      </c>
+      <c r="V21" s="4">
+        <v>1.085</v>
+      </c>
+      <c r="W21" s="4">
+        <v>-3.8929999999999998</v>
+      </c>
+      <c r="Y21" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z21" s="4">
+        <v>1.085</v>
+      </c>
+      <c r="AA21" s="4">
+        <v>-3.8929999999999998</v>
+      </c>
+      <c r="AG21" s="6">
+        <v>1</v>
+      </c>
+      <c r="AH21" s="8"/>
+      <c r="AI21" s="7"/>
+      <c r="AJ21" s="7"/>
+      <c r="AK21" s="7" t="e">
+        <f>AVERAGE(AH21:AJ21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS21" s="6">
+        <v>1</v>
+      </c>
+      <c r="AT21" s="8"/>
+      <c r="AU21" s="7"/>
+      <c r="AV21" s="7"/>
+      <c r="AW21" s="7" t="e">
+        <f>AVERAGE(AT21:AV21)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="13:49" x14ac:dyDescent="0.3">
+      <c r="M22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N22" s="1">
+        <f>AVERAGE(N17:N21)</f>
+        <v>1.1082000000000001</v>
+      </c>
+      <c r="O22" s="1">
+        <f>AVERAGE(O17:O21)</f>
+        <v>-4.8708000000000009</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R22" s="1">
+        <f>AVERAGE(R17:R21)</f>
+        <v>1.1093999999999999</v>
+      </c>
+      <c r="S22" s="1">
+        <f>AVERAGE(S17:S21)</f>
+        <v>-4.9039999999999999</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V22" s="1">
+        <f>AVERAGE(V17:V21)</f>
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="W22" s="1">
+        <f>AVERAGE(W17:W21)</f>
+        <v>-4.7576000000000001</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z22" s="1">
+        <f>AVERAGE(Z17:Z21)</f>
+        <v>1.1004</v>
+      </c>
+      <c r="AA22" s="1">
+        <f>AVERAGE(AA17:AA21)</f>
+        <v>-4.6151999999999997</v>
+      </c>
+      <c r="AG22" s="6">
+        <v>2</v>
+      </c>
+      <c r="AH22" s="7"/>
+      <c r="AI22" s="7"/>
+      <c r="AJ22" s="8"/>
+      <c r="AK22" s="7" t="e">
+        <f>AVERAGE(AH22:AJ22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS22" s="6">
+        <v>2</v>
+      </c>
+      <c r="AT22" s="7"/>
+      <c r="AU22" s="7"/>
+      <c r="AV22" s="8"/>
+      <c r="AW22" s="7" t="e">
+        <f>AVERAGE(AT22:AV22)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="13:49" x14ac:dyDescent="0.3">
+      <c r="AG23" s="6">
+        <v>3</v>
+      </c>
+      <c r="AH23" s="7">
+        <v>1.1659999999999999</v>
+      </c>
+      <c r="AI23" s="8"/>
+      <c r="AJ23" s="7"/>
+      <c r="AK23" s="7">
+        <f>AVERAGE(AH23:AJ23)</f>
+        <v>1.1659999999999999</v>
+      </c>
+      <c r="AS23" s="6">
+        <v>3</v>
+      </c>
+      <c r="AT23" s="7">
+        <v>0.41039999999999999</v>
+      </c>
+      <c r="AU23" s="8"/>
+      <c r="AV23" s="7"/>
+      <c r="AW23" s="7">
+        <f>AVERAGE(AT23:AV23)</f>
+        <v>0.41039999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="13:49" x14ac:dyDescent="0.3">
+      <c r="AG24" s="6">
+        <v>4</v>
+      </c>
+      <c r="AH24" s="7"/>
+      <c r="AI24" s="8"/>
+      <c r="AJ24" s="7"/>
+      <c r="AK24" s="7" t="e">
+        <f>AVERAGE(AH24:AJ24)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS24" s="6">
+        <v>4</v>
+      </c>
+      <c r="AT24" s="7"/>
+      <c r="AU24" s="8"/>
+      <c r="AV24" s="7"/>
+      <c r="AW24" s="7" t="e">
+        <f>AVERAGE(AT24:AV24)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="13:49" x14ac:dyDescent="0.3">
+      <c r="M25" s="1">
+        <v>1</v>
+      </c>
+      <c r="N25" s="4">
+        <v>1.121</v>
+      </c>
+      <c r="O25" s="4">
+        <v>-5.1840000000000002</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>1</v>
+      </c>
+      <c r="R25" s="4">
+        <v>1.121</v>
+      </c>
+      <c r="S25" s="4">
+        <v>-5.1840000000000002</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V25" s="13">
+        <v>1</v>
+      </c>
+      <c r="W25" s="13"/>
+      <c r="X25" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y25" s="13"/>
+      <c r="Z25" s="13">
+        <v>3</v>
+      </c>
+      <c r="AA25" s="13"/>
+      <c r="AB25" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD25" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG25" s="6">
+        <v>5</v>
+      </c>
+      <c r="AH25" s="8">
+        <v>1.1459999999999999</v>
+      </c>
+      <c r="AI25" s="7">
+        <v>0.83250000000000002</v>
+      </c>
+      <c r="AJ25" s="7">
+        <v>0.76580000000000004</v>
+      </c>
+      <c r="AK25" s="7">
+        <f>AVERAGE(AH25:AJ25)</f>
+        <v>0.91476666666666662</v>
+      </c>
+      <c r="AS25" s="6">
+        <v>5</v>
+      </c>
+      <c r="AT25" s="8">
+        <v>0.41880000000000001</v>
+      </c>
+      <c r="AU25" s="7">
+        <v>0.27029999999999998</v>
+      </c>
+      <c r="AV25" s="7">
+        <v>0.2442</v>
+      </c>
+      <c r="AW25" s="7">
+        <f>AVERAGE(AT25:AV25)</f>
+        <v>0.31109999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="13:49" x14ac:dyDescent="0.3">
+      <c r="M26" s="1">
+        <v>2</v>
+      </c>
+      <c r="N26" s="4">
+        <v>1.0920000000000001</v>
+      </c>
+      <c r="O26" s="4">
+        <v>-4.4569999999999999</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>2</v>
+      </c>
+      <c r="R26" s="4">
+        <v>1.0920000000000001</v>
+      </c>
+      <c r="S26" s="4">
+        <v>-4.4569999999999999</v>
+      </c>
+      <c r="U26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V26" s="1">
+        <v>1.0780000000000001</v>
+      </c>
+      <c r="W26" s="1">
+        <v>-3.5259999999999998</v>
+      </c>
+      <c r="X26" s="1">
+        <v>1.1140000000000001</v>
+      </c>
+      <c r="Y26" s="1">
+        <v>-5.0030000000000001</v>
+      </c>
+      <c r="Z26" s="1">
+        <v>1.1120000000000001</v>
+      </c>
+      <c r="AA26" s="1">
+        <v>-5.2359999999999998</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="AC26" s="1">
+        <v>-5.085</v>
+      </c>
+      <c r="AD26" s="2">
+        <v>1.069</v>
+      </c>
+      <c r="AE26" s="2">
+        <v>-3.0390000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="13:49" x14ac:dyDescent="0.3">
+      <c r="M27" s="1">
+        <v>3</v>
+      </c>
+      <c r="N27" s="4">
+        <v>1.095</v>
+      </c>
+      <c r="O27" s="4">
+        <v>-4.5039999999999996</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>3</v>
+      </c>
+      <c r="R27" s="2">
+        <v>1.113</v>
+      </c>
+      <c r="S27" s="2">
+        <v>-5.1219999999999999</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="V27" s="2">
+        <v>1.141</v>
+      </c>
+      <c r="W27" s="2">
+        <v>-5.6740000000000004</v>
+      </c>
+      <c r="X27" s="2">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="Y27" s="2">
+        <v>-5.1689999999999996</v>
+      </c>
+      <c r="Z27" s="2">
+        <v>1.095</v>
+      </c>
+      <c r="AA27" s="2">
+        <v>-4.5039999999999996</v>
+      </c>
+      <c r="AB27" s="2">
+        <v>1.1679999999999999</v>
+      </c>
+      <c r="AC27" s="2">
+        <v>-6.8390000000000004</v>
+      </c>
+      <c r="AD27" s="2">
+        <v>1.085</v>
+      </c>
+      <c r="AE27" s="2">
+        <v>-3.8929999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="13:49" x14ac:dyDescent="0.3">
+      <c r="M28" s="1">
+        <v>4</v>
+      </c>
+      <c r="N28" s="4">
+        <v>1.109</v>
+      </c>
+      <c r="O28" s="4">
+        <v>-5.0380000000000003</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>4</v>
+      </c>
+      <c r="R28" s="4">
+        <v>1.109</v>
+      </c>
+      <c r="S28" s="4">
+        <v>-5.0380000000000003</v>
+      </c>
+      <c r="U28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V28" s="2">
+        <v>1.121</v>
+      </c>
+      <c r="W28" s="2">
+        <v>-5.1840000000000002</v>
+      </c>
+      <c r="X28" s="2">
+        <v>1.0920000000000001</v>
+      </c>
+      <c r="Y28" s="2">
+        <v>-4.4569999999999999</v>
+      </c>
+      <c r="Z28" s="2">
+        <v>1.113</v>
+      </c>
+      <c r="AA28" s="2">
+        <v>-5.1219999999999999</v>
+      </c>
+      <c r="AB28" s="2">
+        <v>1.109</v>
+      </c>
+      <c r="AC28" s="2">
+        <v>-5.0380000000000003</v>
+      </c>
+      <c r="AD28" s="2">
+        <v>1.089</v>
+      </c>
+      <c r="AE28" s="2">
+        <v>-4.0359999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="13:49" x14ac:dyDescent="0.3">
+      <c r="M29" s="1">
+        <v>5</v>
+      </c>
+      <c r="N29" s="2">
+        <v>1.089</v>
+      </c>
+      <c r="O29" s="2">
+        <v>-4.0359999999999996</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>5</v>
+      </c>
+      <c r="R29" s="4">
+        <v>1.089</v>
+      </c>
+      <c r="S29" s="4">
+        <v>-4.0359999999999996</v>
+      </c>
+      <c r="V29" s="1">
+        <f t="shared" ref="V29:AE29" si="0">AVERAGE(V26:V28)</f>
+        <v>1.1133333333333335</v>
+      </c>
+      <c r="W29" s="1">
+        <f t="shared" si="0"/>
+        <v>-4.7946666666666671</v>
+      </c>
+      <c r="X29" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1086666666666667</v>
+      </c>
+      <c r="Y29" s="1">
+        <f t="shared" si="0"/>
+        <v>-4.8763333333333341</v>
+      </c>
+      <c r="Z29" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1066666666666667</v>
+      </c>
+      <c r="AA29" s="1">
+        <f t="shared" si="0"/>
+        <v>-4.9539999999999997</v>
+      </c>
+      <c r="AB29" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1276666666666666</v>
+      </c>
+      <c r="AC29" s="1">
+        <f t="shared" si="0"/>
+        <v>-5.6539999999999999</v>
+      </c>
+      <c r="AD29" s="1">
+        <f t="shared" si="0"/>
+        <v>1.081</v>
+      </c>
+      <c r="AE29" s="1">
+        <f t="shared" si="0"/>
+        <v>-3.6560000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="13:49" x14ac:dyDescent="0.3">
+      <c r="M30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N30" s="1">
+        <f>AVERAGE(N25:N29)</f>
+        <v>1.1012</v>
+      </c>
+      <c r="O30" s="1">
+        <f>AVERAGE(O25:O29)</f>
+        <v>-4.6438000000000006</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R30" s="1">
+        <f>AVERAGE(R25:R29)</f>
+        <v>1.1048000000000002</v>
+      </c>
+      <c r="S30" s="1">
+        <f>AVERAGE(S25:S29)</f>
+        <v>-4.7674000000000003</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="AY10:BC10"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="X25:Y25"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="AS19:AW19"/>
+    <mergeCell ref="AG1:AK1"/>
+    <mergeCell ref="AM1:AQ1"/>
+    <mergeCell ref="AG10:AK10"/>
+    <mergeCell ref="AM10:AQ10"/>
+    <mergeCell ref="AG19:AK19"/>
+    <mergeCell ref="AS10:AW10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>